<commit_message>
1st Test case Review and Ratings added
</commit_message>
<xml_diff>
--- a/msupply_5/src/test/resources/Locators.xlsx
+++ b/msupply_5/src/test/resources/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -97,7 +97,7 @@
     <t>MobileNumberField_Xpath</t>
   </si>
   <si>
-    <t>//*[@id='magestore-sociallogin-popup-email']</t>
+    <t>//input[@name='socialogin_email']</t>
   </si>
   <si>
     <t>PasswordField_Xpath</t>
@@ -110,6 +110,60 @@
   </si>
   <si>
     <t>//*[@id='magestore-button-sociallogin']</t>
+  </si>
+  <si>
+    <t>Login_For_Review_And_Rating_LinkText</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>Rating_Text_Xpath</t>
+  </si>
+  <si>
+    <t>(//form[@id='review-form']//div[2])[1]/h5</t>
+  </si>
+  <si>
+    <t>Review_Text_Xpath</t>
+  </si>
+  <si>
+    <t>(//form[@id='review-form']//div[2])[1]/ul/h5</t>
+  </si>
+  <si>
+    <t>Rating_Stars_Xpath</t>
+  </si>
+  <si>
+    <t>(//form[@id='review-form']//div[2])[1]/div[1]/ul/li</t>
+  </si>
+  <si>
+    <t>Empty_Rating_Stars_Xpath</t>
+  </si>
+  <si>
+    <t>(//form[@id='review-form']//div[2])[1]/div[1]/div[2]/input</t>
+  </si>
+  <si>
+    <t>Review_Title_Label_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='review-form']/fieldset/div[2]/ul/li[1]/label</t>
+  </si>
+  <si>
+    <t>Review_Title_TextBox_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='summary_field']</t>
+  </si>
+  <si>
+    <t>Review_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='review-form']/fieldset/div[2]/ul/li[2]/label</t>
+  </si>
+  <si>
+    <t>Review_TextBox_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='review_field']</t>
   </si>
 </sst>
 </file>
@@ -336,23 +390,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="106.239795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="105.025510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -444,35 +498,107 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reviews and ratings Test Case 1 and 2 Completed
</commit_message>
<xml_diff>
--- a/msupply_5/src/test/resources/Locators.xlsx
+++ b/msupply_5/src/test/resources/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>//*[@id='review_field']</t>
+  </si>
+  <si>
+    <t>Submit_Review_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='review-form']/fieldset/div[2]/div[2]/button</t>
+  </si>
+  <si>
+    <t>Review_Title_Textbox_ErrorMsg_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='advice-required-entry-summary_field']</t>
+  </si>
+  <si>
+    <t>Review_Textbox_ErrorMsg_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='advice-required-entry-review_field']</t>
   </si>
 </sst>
 </file>
@@ -173,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -210,12 +228,6 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,7 +284,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,10 +318,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,23 +398,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="105.025510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="103.80612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -530,75 +538,99 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="8" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testcase1 and TestCase2 completed TestCase7 in progress
</commit_message>
<xml_diff>
--- a/msupply_5/src/test/resources/Locators.xlsx
+++ b/msupply_5/src/test/resources/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Key</t>
   </si>
@@ -182,6 +182,36 @@
   </si>
   <si>
     <t>//*[@id='advice-required-entry-review_field']</t>
+  </si>
+  <si>
+    <t>SuccessMessage_Xpath</t>
+  </si>
+  <si>
+    <t>//ul[@class='messages']/li/ul/li</t>
+  </si>
+  <si>
+    <t>HomePage_Account_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='lnkAccount']/a</t>
+  </si>
+  <si>
+    <t>HomePage_Login_Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id='divAccount']/ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>No_Of_Customer_Reviews_Xpath</t>
+  </si>
+  <si>
+    <t>(//div[@class='col-lg-9 customer_reviews pull-right']/div)</t>
+  </si>
+  <si>
+    <t>Review_Date_Xpath</t>
+  </si>
+  <si>
+    <t>(//li[@class='rvw_title block clear']/div)[2]</t>
   </si>
 </sst>
 </file>
@@ -191,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -228,6 +258,12 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -284,7 +320,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,6 +354,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,23 +438,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="103.80612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="73.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="102.729591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -610,27 +650,67 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="8" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reviews and Ratings Testcase 1,2 and 7(in progress)
</commit_message>
<xml_diff>
--- a/msupply_5/src/test/resources/Locators.xlsx
+++ b/msupply_5/src/test/resources/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Key</t>
   </si>
@@ -85,7 +85,7 @@
     <t>Write_Review_Link_Xpath</t>
   </si>
   <si>
-    <t>Write a review</t>
+    <t>Write Your Review</t>
   </si>
   <si>
     <t>Login_For_Review_And_Rating_Xpath</t>
@@ -211,7 +211,13 @@
     <t>Review_Date_Xpath</t>
   </si>
   <si>
-    <t>(//li[@class='rvw_title block clear']/div)[2]</t>
+    <t>((//li[@class='rvw_title block clear']/div[2]))</t>
+  </si>
+  <si>
+    <t>No_of_Customer_Reviews_DetailsPage_Xpath</t>
+  </si>
+  <si>
+    <t>//p[@class='rating-links customreview']/a[1]</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -541,7 +547,7 @@
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -711,6 +717,14 @@
       </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Home page sliders testscript
</commit_message>
<xml_diff>
--- a/msupply_5/src/test/resources/Locators.xlsx
+++ b/msupply_5/src/test/resources/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="526">
   <si>
     <t>Key</t>
   </si>
@@ -1490,9 +1490,6 @@
   </si>
   <si>
     <t>//*[@id='btnLogout']</t>
-  </si>
-  <si>
-    <t>MainCategory_Xpath</t>
   </si>
   <si>
     <t>Shopping Kart Page</t>
@@ -1873,18 +1870,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C279"/>
+  <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A240" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C255" activeCellId="0" sqref="C255"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A249" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A280" activeCellId="0" sqref="A280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.7193877551021"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4677,206 +4674,206 @@
         <v>489</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="5" t="s">
+    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="B255" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C255" s="5" t="s">
-        <v>318</v>
-      </c>
+      <c r="B255" s="9"/>
+      <c r="C255" s="10"/>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="7" t="s">
+      <c r="A256" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="B256" s="9"/>
-      <c r="C256" s="10"/>
+      <c r="B256" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C257" s="5" t="s">
+      <c r="A257" s="11" t="s">
         <v>493</v>
       </c>
+      <c r="B257" s="8"/>
+      <c r="C257" s="1"/>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="11" t="s">
+      <c r="A258" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="B258" s="8"/>
-      <c r="C258" s="1"/>
+      <c r="B258" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="5" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="B260" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C260" s="5" t="s">
+      <c r="A260" s="7" t="s">
         <v>498</v>
       </c>
+      <c r="B260" s="9"/>
+      <c r="C260" s="12"/>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="7" t="s">
+      <c r="A261" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="B261" s="9"/>
-      <c r="C261" s="12"/>
+      <c r="B261" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="5" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="5" t="s">
+      <c r="A263" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="B263" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C263" s="5" t="s">
-        <v>498</v>
-      </c>
+      <c r="B263" s="13"/>
+      <c r="C263" s="7"/>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="7" t="s">
+      <c r="A264" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="B264" s="13"/>
-      <c r="C264" s="7"/>
+      <c r="B264" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="5" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="5" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C267" s="5" t="s">
+      <c r="A267" s="7" t="s">
         <v>509</v>
       </c>
+      <c r="B267" s="9"/>
+      <c r="C267" s="12"/>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="7" t="s">
+      <c r="A268" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="B268" s="9"/>
-      <c r="C268" s="12"/>
+      <c r="B268" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="B269" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C269" s="5" t="s">
+      <c r="A269" s="7" t="s">
         <v>512</v>
       </c>
+      <c r="B269" s="13"/>
+      <c r="C269" s="7"/>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="7" t="s">
+      <c r="A270" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="B270" s="13"/>
-      <c r="C270" s="7"/>
+      <c r="B270" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C270" s="14" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="B271" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C271" s="14" t="s">
+      <c r="A271" s="7" t="s">
         <v>515</v>
       </c>
+      <c r="B271" s="15"/>
+      <c r="C271" s="15"/>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="7" t="s">
+      <c r="A272" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="B272" s="15"/>
-      <c r="C272" s="15"/>
+      <c r="B272" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="B273" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C273" s="3" t="s">
+      <c r="A273" s="15"/>
+      <c r="B273" s="15"/>
+      <c r="C273" s="15"/>
+    </row>
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="5" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="15"/>
-      <c r="B274" s="15"/>
-      <c r="C274" s="15"/>
-    </row>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="5" t="s">
+      <c r="B274" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C274" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="B275" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C275" s="5" t="s">
+    </row>
+    <row r="275" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="16" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="276" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="16" t="s">
+    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
         <v>521</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4887,31 +4884,21 @@
         <v>4</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
         <v>525</v>
       </c>
-      <c r="B279" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C279" s="0" t="s">
-        <v>526</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>